<commit_message>
chore: commit all changes (assets via LFS, track output/img, notebooks)
</commit_message>
<xml_diff>
--- a/theodoihangngay.xlsx
+++ b/theodoihangngay.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,26 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7616438356164383</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'c_w': 0.25447054029049226, 'c_s': 1.8568662619089953, 'den_mid': 0.46439117657448753, 'den_high': 0.6446772564277745, 'low_thres': 0.6399957717850465, 'high_thres': 0.6979598879442052, 'p_base_h': 0.20097534714976714, 'c_r': 1.1609414221653496, 'c_t': 1.082500226109699, 't_ref_c': 33.17811951296828, 't_scale': 5.030357500017056, 'rain_win': 3, 'r_ref_mm': 6.6653330727891, 'yama_step': 62, 'c_y': 0.03582999029214878, 'yama_cap': 2.386033787257072, 'burn_steps': 6, 'ember_chance': 0.04340509960691442, 'c_h': 0.024262980583097227, 'h_ref': 79.14251040914458, 'h_scale': 17.568516859786204, 'c_sm': 0.7011653727056256}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Đã thêm độ ẩm không khí (c_h, h_ref, h_scale) và độ ẩm đất (c_sm). So sánh F1 theo trạng thái cuối sau đúng n_t, không dừng sớm.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>